<commit_message>
Added voltage divider Values to Thermister spreadsheet
</commit_message>
<xml_diff>
--- a/ThermisterTTC103.xlsx
+++ b/ThermisterTTC103.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\school\College\Sem 5\Embedded\Lab\MS2\milestone-2-front-row-squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC0A561-36F3-4C91-B260-7E7DD270389C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C894FC8-33D3-4306-8641-DA912552F5D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3B8B9557-4AC8-4DDE-8A78-C31AB3DB3422}"/>
+    <workbookView xWindow="5760" yWindow="3246" windowWidth="17280" windowHeight="8994" xr2:uid="{3B8B9557-4AC8-4DDE-8A78-C31AB3DB3422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Temp</t>
   </si>
   <si>
     <t>Resistance</t>
+  </si>
+  <si>
+    <t>Voltage Divider Low</t>
   </si>
 </sst>
 </file>
@@ -1435,148 +1438,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41279EC-6228-4CFC-A1CF-733EA1FFCBC1}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="128" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>-30</v>
       </c>
       <c r="B2">
         <v>150000</v>
       </c>
+      <c r="M2">
+        <f>3.3*B2/(B2+10000)</f>
+        <v>3.09375</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>-20</v>
       </c>
       <c r="B3">
         <v>80000</v>
       </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M17" si="0">3.3*B3/(B3+10000)</f>
+        <v>2.9333333333333331</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>-10</v>
       </c>
       <c r="B4">
         <v>50000</v>
       </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
         <v>30000</v>
       </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>2.4750000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6">
         <v>19500</v>
       </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>2.18135593220339</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="B7">
         <v>12000</v>
       </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>25</v>
       </c>
       <c r="B8">
         <v>10000</v>
       </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>30</v>
       </c>
       <c r="B9">
         <v>8000</v>
       </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1.4666666666666666</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>40</v>
       </c>
       <c r="B10">
         <v>5500</v>
       </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>1.1709677419354838</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>50</v>
       </c>
       <c r="B11">
         <v>4000</v>
       </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0.94285714285714284</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>60</v>
       </c>
       <c r="B12">
         <v>2700</v>
       </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0.7015748031496063</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>70</v>
       </c>
       <c r="B13">
         <v>2000</v>
       </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>80</v>
       </c>
       <c r="B14">
         <v>1500</v>
       </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0.43043478260869567</v>
+      </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>90</v>
       </c>
       <c r="B15">
         <v>1000</v>
       </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>100</v>
       </c>
       <c r="B16">
         <v>800</v>
       </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0.24444444444444444</v>
+      </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>120</v>
       </c>
       <c r="B17">
         <v>470</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>0.1481375358166189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel thermister sheet
</commit_message>
<xml_diff>
--- a/ThermisterTTC103.xlsx
+++ b/ThermisterTTC103.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\school\College\Sem 5\Embedded\Lab\MS2\milestone-2-front-row-squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C894FC8-33D3-4306-8641-DA912552F5D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E5CC31-7D53-405C-B42D-50EEF02902E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3246" windowWidth="17280" windowHeight="8994" xr2:uid="{3B8B9557-4AC8-4DDE-8A78-C31AB3DB3422}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3B8B9557-4AC8-4DDE-8A78-C31AB3DB3422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>Resistance</t>
   </si>
   <si>
-    <t>Voltage Divider Low</t>
+    <t>Voltage Divider</t>
   </si>
 </sst>
 </file>
@@ -1438,214 +1438,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41279EC-6228-4CFC-A1CF-733EA1FFCBC1}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>-30</v>
       </c>
       <c r="B2">
         <v>150000</v>
       </c>
-      <c r="M2">
+      <c r="K2">
         <f>3.3*B2/(B2+10000)</f>
         <v>3.09375</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>-20</v>
       </c>
       <c r="B3">
         <v>80000</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M17" si="0">3.3*B3/(B3+10000)</f>
+      <c r="K3">
+        <f>3.3*B3/(B3+10000)</f>
         <v>2.9333333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>-10</v>
       </c>
       <c r="B4">
         <v>50000</v>
       </c>
-      <c r="M4">
-        <f t="shared" si="0"/>
+      <c r="K4">
+        <f>3.3*B4/(B4+10000)</f>
         <v>2.75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
         <v>30000</v>
       </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
+      <c r="K5">
+        <f>3.3*B5/(B5+10000)</f>
         <v>2.4750000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6">
         <v>19500</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
+      <c r="K6">
+        <f>3.3*B6/(B6+10000)</f>
         <v>2.18135593220339</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="B7">
         <v>12000</v>
       </c>
-      <c r="M7">
-        <f t="shared" si="0"/>
+      <c r="K7">
+        <f>3.3*B7/(B7+10000)</f>
         <v>1.8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>25</v>
       </c>
       <c r="B8">
         <v>10000</v>
       </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
+      <c r="K8">
+        <f>3.3*B8/(B8+10000)</f>
         <v>1.65</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>30</v>
       </c>
       <c r="B9">
         <v>8000</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
+      <c r="K9">
+        <f>3.3*B9/(B9+10000)</f>
         <v>1.4666666666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>40</v>
       </c>
       <c r="B10">
         <v>5500</v>
       </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
+      <c r="K10">
+        <f>3.3*B10/(B10+10000)</f>
         <v>1.1709677419354838</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>50</v>
       </c>
       <c r="B11">
         <v>4000</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="0"/>
+      <c r="K11">
+        <f>3.3*B11/(B11+10000)</f>
         <v>0.94285714285714284</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>60</v>
       </c>
       <c r="B12">
         <v>2700</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
+      <c r="K12">
+        <f>3.3*B12/(B12+10000)</f>
         <v>0.7015748031496063</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>70</v>
       </c>
       <c r="B13">
         <v>2000</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="0"/>
+      <c r="K13">
+        <f>3.3*B13/(B13+10000)</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>80</v>
       </c>
       <c r="B14">
         <v>1500</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="0"/>
+      <c r="K14">
+        <f>3.3*B14/(B14+10000)</f>
         <v>0.43043478260869567</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>90</v>
       </c>
       <c r="B15">
         <v>1000</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
+      <c r="K15">
+        <f>3.3*B15/(B15+10000)</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>100</v>
       </c>
       <c r="B16">
         <v>800</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="0"/>
+      <c r="K16">
+        <f>3.3*B16/(B16+10000)</f>
         <v>0.24444444444444444</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>120</v>
       </c>
       <c r="B17">
         <v>470</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="0"/>
+      <c r="K17">
+        <f>3.3*B17/(B17+10000)</f>
         <v>0.1481375358166189</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated thermister sheet again
</commit_message>
<xml_diff>
--- a/ThermisterTTC103.xlsx
+++ b/ThermisterTTC103.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\school\College\Sem 5\Embedded\Lab\MS2\milestone-2-front-row-squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E5CC31-7D53-405C-B42D-50EEF02902E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9419F4F0-3F71-48E2-A9E6-5966951DFAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3B8B9557-4AC8-4DDE-8A78-C31AB3DB3422}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Temp</t>
   </si>
@@ -40,6 +42,9 @@
   </si>
   <si>
     <t>Voltage Divider</t>
+  </si>
+  <si>
+    <t>Room Temp</t>
   </si>
 </sst>
 </file>
@@ -1438,15 +1443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41279EC-6228-4CFC-A1CF-733EA1FFCBC1}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1457,7 +1462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>-30</v>
       </c>
@@ -1469,7 +1474,7 @@
         <v>3.09375</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>-20</v>
       </c>
@@ -1477,11 +1482,11 @@
         <v>80000</v>
       </c>
       <c r="K3">
-        <f>3.3*B3/(B3+10000)</f>
+        <f t="shared" ref="K2:K17" si="0">3.3*B3/(B3+10000)</f>
         <v>2.9333333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>-10</v>
       </c>
@@ -1489,11 +1494,11 @@
         <v>50000</v>
       </c>
       <c r="K4">
-        <f>3.3*B4/(B4+10000)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1501,11 +1506,11 @@
         <v>30000</v>
       </c>
       <c r="K5">
-        <f>3.3*B5/(B5+10000)</f>
+        <f t="shared" si="0"/>
         <v>2.4750000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1513,11 +1518,11 @@
         <v>19500</v>
       </c>
       <c r="K6">
-        <f>3.3*B6/(B6+10000)</f>
+        <f t="shared" si="0"/>
         <v>2.18135593220339</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>20</v>
       </c>
@@ -1525,11 +1530,11 @@
         <v>12000</v>
       </c>
       <c r="K7">
-        <f>3.3*B7/(B7+10000)</f>
+        <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>25</v>
       </c>
@@ -1537,11 +1542,14 @@
         <v>10000</v>
       </c>
       <c r="K8">
-        <f>3.3*B8/(B8+10000)</f>
+        <f t="shared" si="0"/>
         <v>1.65</v>
       </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>30</v>
       </c>
@@ -1549,11 +1557,11 @@
         <v>8000</v>
       </c>
       <c r="K9">
-        <f>3.3*B9/(B9+10000)</f>
+        <f t="shared" si="0"/>
         <v>1.4666666666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>40</v>
       </c>
@@ -1561,11 +1569,11 @@
         <v>5500</v>
       </c>
       <c r="K10">
-        <f>3.3*B10/(B10+10000)</f>
+        <f t="shared" si="0"/>
         <v>1.1709677419354838</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>50</v>
       </c>
@@ -1573,11 +1581,11 @@
         <v>4000</v>
       </c>
       <c r="K11">
-        <f>3.3*B11/(B11+10000)</f>
+        <f t="shared" si="0"/>
         <v>0.94285714285714284</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>60</v>
       </c>
@@ -1585,11 +1593,11 @@
         <v>2700</v>
       </c>
       <c r="K12">
-        <f>3.3*B12/(B12+10000)</f>
+        <f t="shared" si="0"/>
         <v>0.7015748031496063</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>70</v>
       </c>
@@ -1597,11 +1605,11 @@
         <v>2000</v>
       </c>
       <c r="K13">
-        <f>3.3*B13/(B13+10000)</f>
+        <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>80</v>
       </c>
@@ -1609,11 +1617,11 @@
         <v>1500</v>
       </c>
       <c r="K14">
-        <f>3.3*B14/(B14+10000)</f>
+        <f t="shared" si="0"/>
         <v>0.43043478260869567</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>90</v>
       </c>
@@ -1621,11 +1629,11 @@
         <v>1000</v>
       </c>
       <c r="K15">
-        <f>3.3*B15/(B15+10000)</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>100</v>
       </c>
@@ -1633,7 +1641,7 @@
         <v>800</v>
       </c>
       <c r="K16">
-        <f>3.3*B16/(B16+10000)</f>
+        <f t="shared" si="0"/>
         <v>0.24444444444444444</v>
       </c>
     </row>
@@ -1645,7 +1653,7 @@
         <v>470</v>
       </c>
       <c r="K17">
-        <f>3.3*B17/(B17+10000)</f>
+        <f t="shared" si="0"/>
         <v>0.1481375358166189</v>
       </c>
     </row>

</xml_diff>